<commit_message>
3.3.1.1 --> 3.4.0 update ctrl-settings/BAEPAbCiPC (all fuels affected by production costs)
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
+++ b/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\ctrl-settings\BAEPAbCiPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\eps-eu\InputData\ctrl-settings\BAEPAbCiPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821543C2-567D-4203-BA9D-917EA0EB3665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781E1C5F-9A32-453D-89FC-98FA9052C77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="435" windowWidth="23595" windowHeight="16230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="120" windowWidth="14400" windowHeight="9690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -196,7 +196,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,16 +478,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,52 +495,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -559,44 +558,46 @@
   </sheetPr>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -604,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -612,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -620,7 +621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -628,63 +629,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -692,39 +693,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -732,11 +733,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to US develop branch #476b0b3 on 9/3/24
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
+++ b/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\BAEPAbCiPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ctrl-settings\BAEPAbCiPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF24940A-FBE5-400B-A056-81583C89D2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEA0A00-D6A6-4D26-8247-961C9C80FF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +702,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>